<commit_message>
sesion7 formularios sesiones y htaccess
</commit_message>
<xml_diff>
--- a/SILABO_2015A TSI553 Ambientes No Propietarios_Salvador Edwin.xlsx
+++ b/SILABO_2015A TSI553 Ambientes No Propietarios_Salvador Edwin.xlsx
@@ -468,10 +468,10 @@
     Comentarios, Sintaxis, Variables, Operadores, Asignación, Tipos, Constantes y constantes predefinidas</t>
   </si>
   <si>
-    <t>pregumtas sobre clase anterior</t>
-  </si>
-  <si>
     <t>Preguntas semanales</t>
+  </si>
+  <si>
+    <t>preguntas sobre clase anterior</t>
   </si>
 </sst>
 </file>
@@ -951,52 +951,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1005,88 +960,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1100,6 +980,126 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1523,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117:F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1541,47 +1541,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="83.25" customHeight="1">
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="2" spans="1:9" ht="18.75">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="4" spans="1:9" ht="18.75">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="1:9" ht="18.75">
       <c r="A5" s="3"/>
@@ -1595,104 +1595,104 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="32"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="35"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="4"/>
@@ -1706,252 +1706,252 @@
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="35"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="32"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="35"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="4"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="32"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="35"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="32"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="78" customHeight="1">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="70"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="73"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1">
       <c r="A30" s="4"/>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="29"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1">
       <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="32"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="35"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
       <c r="A35" s="4"/>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="32"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="53"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1">
-      <c r="A37" s="33">
+      <c r="A37" s="65">
         <v>3</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="35"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
       <c r="A38" s="4"/>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="32"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="53"/>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="67"/>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1">
       <c r="A41" s="4"/>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="32"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
@@ -1974,17 +1974,17 @@
       <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="32"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="53"/>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1">
       <c r="A46" s="5" t="s">
@@ -2009,7 +2009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" customHeight="1">
+    <row r="47" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="4"/>
     </row>
     <row r="48" spans="1:9" ht="173.25" hidden="1" customHeight="1">
@@ -2078,31 +2078,31 @@
       <c r="H53" s="11"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A54" s="30" t="s">
+    <row r="54" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
+      <c r="A54" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="32"/>
-    </row>
-    <row r="55" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A55" s="33" t="s">
+      <c r="B54" s="52"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="53"/>
+    </row>
+    <row r="55" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1">
+      <c r="A55" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="35"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="66"/>
+      <c r="G55" s="66"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="67"/>
     </row>
     <row r="56" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A56" s="4"/>
@@ -2116,128 +2116,128 @@
       <c r="I56"/>
     </row>
     <row r="57" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="32"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="53"/>
     </row>
     <row r="58" spans="1:10" ht="30" customHeight="1">
-      <c r="A58" s="33"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="35"/>
+      <c r="A58" s="65"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="67"/>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1">
       <c r="A59" s="4"/>
     </row>
     <row r="60" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="29"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="50"/>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1">
       <c r="A61" s="4"/>
     </row>
     <row r="62" spans="1:10" ht="45" customHeight="1">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="36" t="s">
+      <c r="B62" s="69"/>
+      <c r="C62" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="36" t="s">
+      <c r="D62" s="70"/>
+      <c r="E62" s="70"/>
+      <c r="F62" s="70"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="I62" s="37"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:10" ht="121.5" customHeight="1">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="41" t="s">
+      <c r="B63" s="64"/>
+      <c r="C63" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="41"/>
-      <c r="I63" s="42"/>
-      <c r="J63" s="42"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
     </row>
     <row r="64" spans="1:10" ht="85.5" customHeight="1">
-      <c r="A64" s="39" t="s">
+      <c r="A64" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="41" t="s">
+      <c r="B64" s="64"/>
+      <c r="C64" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="42"/>
-      <c r="J64" s="42"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
     </row>
     <row r="65" spans="1:10" ht="61.5" customHeight="1">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="40"/>
-      <c r="C65" s="41" t="s">
+      <c r="B65" s="64"/>
+      <c r="C65" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="42"/>
-      <c r="J65" s="42"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1">
       <c r="A66" s="4"/>
     </row>
     <row r="67" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="29"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="49"/>
+      <c r="E67" s="49"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="50"/>
     </row>
     <row r="68" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A68" s="4"/>
@@ -2251,178 +2251,178 @@
       <c r="I68"/>
     </row>
     <row r="69" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A69" s="30" t="s">
+      <c r="A69" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="32"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="52"/>
+      <c r="F69" s="52"/>
+      <c r="G69" s="52"/>
+      <c r="H69" s="52"/>
+      <c r="I69" s="53"/>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1">
       <c r="A70" s="4"/>
     </row>
     <row r="71" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B71" s="45"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="45"/>
-      <c r="H71" s="45"/>
-      <c r="I71" s="46"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
+      <c r="I71" s="56"/>
     </row>
     <row r="72" spans="1:10" ht="409.5" customHeight="1" thickBot="1">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="49"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="59"/>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="31"/>
-      <c r="I74" s="32"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="52"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="52"/>
+      <c r="H74" s="52"/>
+      <c r="I74" s="53"/>
     </row>
     <row r="75" spans="1:10" ht="62.25" customHeight="1">
-      <c r="A75" s="50" t="s">
+      <c r="A75" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="51"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="51"/>
-      <c r="F75" s="51"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="51"/>
-      <c r="I75" s="52"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="62"/>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1">
       <c r="A76" s="4"/>
     </row>
     <row r="77" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A77" s="30" t="s">
+      <c r="A77" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B77" s="31"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="31"/>
-      <c r="I77" s="32"/>
+      <c r="B77" s="52"/>
+      <c r="C77" s="52"/>
+      <c r="D77" s="52"/>
+      <c r="E77" s="52"/>
+      <c r="F77" s="52"/>
+      <c r="G77" s="52"/>
+      <c r="H77" s="52"/>
+      <c r="I77" s="53"/>
     </row>
     <row r="78" spans="1:10" s="1" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A78" s="50" t="s">
+      <c r="A78" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="B78" s="51"/>
-      <c r="C78" s="51"/>
-      <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="51"/>
-      <c r="G78" s="51"/>
-      <c r="H78" s="51"/>
-      <c r="I78" s="52"/>
+      <c r="B78" s="61"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="61"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="62"/>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1">
       <c r="A79" s="4"/>
     </row>
     <row r="80" spans="1:10" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A80" s="30" t="s">
+      <c r="A80" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="31"/>
-      <c r="I80" s="32"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="52"/>
+      <c r="E80" s="52"/>
+      <c r="F80" s="52"/>
+      <c r="G80" s="52"/>
+      <c r="H80" s="52"/>
+      <c r="I80" s="53"/>
     </row>
     <row r="81" spans="1:9" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A81" s="53" t="s">
+      <c r="A81" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="54"/>
-      <c r="C81" s="54"/>
-      <c r="D81" s="54"/>
-      <c r="E81" s="54"/>
-      <c r="F81" s="54"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="54"/>
-      <c r="I81" s="55"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="46"/>
+      <c r="F81" s="46"/>
+      <c r="G81" s="46"/>
+      <c r="H81" s="46"/>
+      <c r="I81" s="47"/>
     </row>
     <row r="82" spans="1:9" ht="15" customHeight="1">
       <c r="A82" s="4"/>
     </row>
     <row r="83" spans="1:9" s="1" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A83" s="56" t="s">
+      <c r="A83" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B83" s="56"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="56"/>
-      <c r="F83" s="56"/>
-      <c r="G83" s="56"/>
-      <c r="H83" s="56"/>
-      <c r="I83" s="56"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="39"/>
+      <c r="I83" s="39"/>
     </row>
     <row r="84" spans="1:9" ht="69" customHeight="1">
-      <c r="A84" s="57" t="s">
+      <c r="A84" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B84" s="58"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
-      <c r="I84" s="59"/>
+      <c r="B84" s="41"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="41"/>
+      <c r="F84" s="41"/>
+      <c r="G84" s="41"/>
+      <c r="H84" s="41"/>
+      <c r="I84" s="42"/>
     </row>
     <row r="85" spans="1:9" ht="15" customHeight="1">
       <c r="A85" s="4"/>
     </row>
     <row r="86" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A86" s="56" t="s">
+      <c r="A86" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B86" s="56"/>
-      <c r="C86" s="56"/>
-      <c r="D86" s="56"/>
-      <c r="E86" s="56"/>
-      <c r="F86" s="56"/>
-      <c r="G86" s="56"/>
-      <c r="H86" s="56"/>
-      <c r="I86" s="56"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="39"/>
     </row>
     <row r="87" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A87" s="4"/>
@@ -2439,14 +2439,14 @@
       <c r="A88" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B88" s="60" t="s">
+      <c r="B88" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="C88" s="60"/>
-      <c r="D88" s="60"/>
-      <c r="E88" s="60"/>
-      <c r="F88" s="60"/>
-      <c r="G88" s="60"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
       <c r="H88" s="14" t="s">
         <v>49</v>
       </c>
@@ -2456,16 +2456,16 @@
     </row>
     <row r="89" spans="1:9" ht="25.5" customHeight="1">
       <c r="A89" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B89" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B89" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="C89" s="62"/>
-      <c r="D89" s="62"/>
-      <c r="E89" s="62"/>
-      <c r="F89" s="62"/>
-      <c r="G89" s="63"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="28"/>
       <c r="H89" s="16">
         <v>10</v>
       </c>
@@ -2477,14 +2477,14 @@
       <c r="A90" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B90" s="61" t="s">
+      <c r="B90" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C90" s="62"/>
-      <c r="D90" s="62"/>
-      <c r="E90" s="62"/>
-      <c r="F90" s="62"/>
-      <c r="G90" s="63"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="28"/>
       <c r="H90" s="16">
         <v>20</v>
       </c>
@@ -2496,14 +2496,14 @@
       <c r="A91" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B91" s="61" t="s">
+      <c r="B91" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C91" s="62"/>
-      <c r="D91" s="62"/>
-      <c r="E91" s="62"/>
-      <c r="F91" s="62"/>
-      <c r="G91" s="63"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="28"/>
       <c r="H91" s="16">
         <v>40</v>
       </c>
@@ -2515,14 +2515,14 @@
       <c r="A92" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B92" s="61" t="s">
+      <c r="B92" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C92" s="62"/>
-      <c r="D92" s="62"/>
-      <c r="E92" s="62"/>
-      <c r="F92" s="62"/>
-      <c r="G92" s="63"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="28"/>
       <c r="H92" s="16">
         <v>30</v>
       </c>
@@ -2534,12 +2534,12 @@
       <c r="A93" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B93" s="61"/>
-      <c r="C93" s="62"/>
-      <c r="D93" s="62"/>
-      <c r="E93" s="62"/>
-      <c r="F93" s="62"/>
-      <c r="G93" s="63"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="28"/>
       <c r="H93" s="17">
         <v>1</v>
       </c>
@@ -2548,10 +2548,10 @@
       </c>
     </row>
     <row r="94" spans="1:9" ht="15" customHeight="1">
-      <c r="A94" s="64" t="s">
+      <c r="A94" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B94" s="64"/>
+      <c r="B94" s="43"/>
       <c r="C94" s="18"/>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -2564,30 +2564,30 @@
       <c r="A95" s="4"/>
     </row>
     <row r="96" spans="1:9" ht="67.5" customHeight="1">
-      <c r="A96" s="56" t="s">
+      <c r="A96" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B96" s="56"/>
-      <c r="C96" s="56"/>
-      <c r="D96" s="56"/>
-      <c r="E96" s="56"/>
-      <c r="F96" s="56"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="56"/>
-      <c r="I96" s="56"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="39"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="39"/>
+      <c r="I96" s="39"/>
     </row>
     <row r="97" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A97" s="57" t="s">
+      <c r="A97" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B97" s="58"/>
-      <c r="C97" s="58"/>
-      <c r="D97" s="58"/>
-      <c r="E97" s="58"/>
-      <c r="F97" s="58"/>
-      <c r="G97" s="58"/>
-      <c r="H97" s="58"/>
-      <c r="I97" s="59"/>
+      <c r="B97" s="41"/>
+      <c r="C97" s="41"/>
+      <c r="D97" s="41"/>
+      <c r="E97" s="41"/>
+      <c r="F97" s="41"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="41"/>
+      <c r="I97" s="42"/>
     </row>
     <row r="98" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A98" s="4"/>
@@ -2601,17 +2601,17 @@
       <c r="I98"/>
     </row>
     <row r="99" spans="1:9" ht="15" customHeight="1">
-      <c r="A99" s="56" t="s">
+      <c r="A99" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B99" s="56"/>
-      <c r="C99" s="56"/>
-      <c r="D99" s="56"/>
-      <c r="E99" s="56"/>
-      <c r="F99" s="56"/>
-      <c r="G99" s="56"/>
-      <c r="H99" s="56"/>
-      <c r="I99" s="56"/>
+      <c r="B99" s="39"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39"/>
+      <c r="G99" s="39"/>
+      <c r="H99" s="39"/>
+      <c r="I99" s="39"/>
     </row>
     <row r="100" spans="1:9" ht="37.5" customHeight="1">
       <c r="A100" s="4"/>
@@ -2623,17 +2623,17 @@
       <c r="B101" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C101" s="60" t="s">
+      <c r="C101" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D101" s="60"/>
-      <c r="E101" s="60"/>
-      <c r="F101" s="60"/>
-      <c r="G101" s="60" t="s">
+      <c r="D101" s="44"/>
+      <c r="E101" s="44"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="H101" s="60"/>
-      <c r="I101" s="60"/>
+      <c r="H101" s="44"/>
+      <c r="I101" s="44"/>
     </row>
     <row r="102" spans="1:9" ht="107.25" customHeight="1">
       <c r="A102" s="16">
@@ -2642,17 +2642,17 @@
       <c r="B102" s="20">
         <v>42101</v>
       </c>
-      <c r="C102" s="41" t="s">
+      <c r="C102" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D102" s="42"/>
-      <c r="E102" s="42"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="65" t="s">
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="30"/>
+      <c r="G102" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="H102" s="65"/>
-      <c r="I102" s="65"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
     </row>
     <row r="103" spans="1:9" ht="63.75" customHeight="1">
       <c r="A103" s="16">
@@ -2661,17 +2661,17 @@
       <c r="B103" s="20">
         <v>42108</v>
       </c>
-      <c r="C103" s="41" t="s">
+      <c r="C103" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D103" s="42"/>
-      <c r="E103" s="42"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="65" t="s">
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="30"/>
+      <c r="G103" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H103" s="65"/>
-      <c r="I103" s="65"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
     </row>
     <row r="104" spans="1:9" ht="66.75" customHeight="1">
       <c r="A104" s="16">
@@ -2680,17 +2680,17 @@
       <c r="B104" s="20">
         <v>42115</v>
       </c>
-      <c r="C104" s="41" t="s">
+      <c r="C104" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D104" s="42"/>
-      <c r="E104" s="42"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="65" t="s">
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="30"/>
+      <c r="G104" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H104" s="65"/>
-      <c r="I104" s="65"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
     </row>
     <row r="105" spans="1:9" ht="75.75" customHeight="1">
       <c r="A105" s="16">
@@ -2699,17 +2699,17 @@
       <c r="B105" s="20">
         <v>42122</v>
       </c>
-      <c r="C105" s="74" t="s">
+      <c r="C105" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="76"/>
-      <c r="G105" s="65" t="s">
+      <c r="D105" s="35"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="36"/>
+      <c r="G105" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H105" s="65"/>
-      <c r="I105" s="65"/>
+      <c r="H105" s="29"/>
+      <c r="I105" s="29"/>
     </row>
     <row r="106" spans="1:9" ht="45.75" customHeight="1">
       <c r="A106" s="16">
@@ -2718,17 +2718,17 @@
       <c r="B106" s="20">
         <v>42129</v>
       </c>
-      <c r="C106" s="41" t="s">
+      <c r="C106" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D106" s="42"/>
-      <c r="E106" s="42"/>
-      <c r="F106" s="43"/>
-      <c r="G106" s="65" t="s">
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="30"/>
+      <c r="G106" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H106" s="65"/>
-      <c r="I106" s="65"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
     </row>
     <row r="107" spans="1:9" ht="80.25" customHeight="1">
       <c r="A107" s="16">
@@ -2737,17 +2737,17 @@
       <c r="B107" s="20">
         <v>42136</v>
       </c>
-      <c r="C107" s="41" t="s">
+      <c r="C107" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D107" s="42"/>
-      <c r="E107" s="42"/>
-      <c r="F107" s="43"/>
-      <c r="G107" s="65" t="s">
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="30"/>
+      <c r="G107" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H107" s="65"/>
-      <c r="I107" s="65"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
     </row>
     <row r="108" spans="1:9" ht="73.5" customHeight="1">
       <c r="A108" s="16">
@@ -2756,17 +2756,17 @@
       <c r="B108" s="20">
         <v>42143</v>
       </c>
-      <c r="C108" s="41" t="s">
+      <c r="C108" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="D108" s="42"/>
-      <c r="E108" s="42"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="65" t="s">
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="30"/>
+      <c r="G108" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H108" s="65"/>
-      <c r="I108" s="65"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
     </row>
     <row r="109" spans="1:9" ht="60" customHeight="1">
       <c r="A109" s="16">
@@ -2775,17 +2775,17 @@
       <c r="B109" s="20">
         <v>42150</v>
       </c>
-      <c r="C109" s="41" t="s">
+      <c r="C109" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="D109" s="42"/>
-      <c r="E109" s="42"/>
-      <c r="F109" s="43"/>
-      <c r="G109" s="65" t="s">
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="30"/>
+      <c r="G109" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H109" s="65"/>
-      <c r="I109" s="65"/>
+      <c r="H109" s="29"/>
+      <c r="I109" s="29"/>
     </row>
     <row r="110" spans="1:9" ht="51.75" customHeight="1">
       <c r="A110" s="16">
@@ -2794,17 +2794,17 @@
       <c r="B110" s="20">
         <v>42157</v>
       </c>
-      <c r="C110" s="41" t="s">
+      <c r="C110" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D110" s="42"/>
-      <c r="E110" s="42"/>
-      <c r="F110" s="43"/>
-      <c r="G110" s="65" t="s">
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="30"/>
+      <c r="G110" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="H110" s="65"/>
-      <c r="I110" s="65"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
     </row>
     <row r="111" spans="1:9" ht="20.25" customHeight="1">
       <c r="A111" s="16">
@@ -2813,17 +2813,17 @@
       <c r="B111" s="20">
         <v>42164</v>
       </c>
-      <c r="C111" s="41" t="s">
+      <c r="C111" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D111" s="42"/>
-      <c r="E111" s="42"/>
-      <c r="F111" s="43"/>
-      <c r="G111" s="63" t="s">
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="30"/>
+      <c r="G111" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="H111" s="65"/>
-      <c r="I111" s="65"/>
+      <c r="H111" s="29"/>
+      <c r="I111" s="29"/>
     </row>
     <row r="112" spans="1:9" ht="20.25" customHeight="1">
       <c r="A112" s="16">
@@ -2832,17 +2832,17 @@
       <c r="B112" s="20">
         <v>42171</v>
       </c>
-      <c r="C112" s="41" t="s">
+      <c r="C112" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D112" s="42"/>
-      <c r="E112" s="42"/>
-      <c r="F112" s="43"/>
-      <c r="G112" s="63" t="s">
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="30"/>
+      <c r="G112" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H112" s="65"/>
-      <c r="I112" s="65"/>
+      <c r="H112" s="29"/>
+      <c r="I112" s="29"/>
     </row>
     <row r="113" spans="1:9" ht="20.25" customHeight="1">
       <c r="A113" s="16">
@@ -2851,17 +2851,17 @@
       <c r="B113" s="20">
         <v>42178</v>
       </c>
-      <c r="C113" s="41" t="s">
+      <c r="C113" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D113" s="42"/>
-      <c r="E113" s="42"/>
-      <c r="F113" s="43"/>
-      <c r="G113" s="63" t="s">
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="30"/>
+      <c r="G113" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H113" s="65"/>
-      <c r="I113" s="65"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
     </row>
     <row r="114" spans="1:9" ht="20.25" customHeight="1">
       <c r="A114" s="16">
@@ -2870,17 +2870,17 @@
       <c r="B114" s="21">
         <v>42185</v>
       </c>
-      <c r="C114" s="41" t="s">
+      <c r="C114" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D114" s="42"/>
-      <c r="E114" s="42"/>
-      <c r="F114" s="43"/>
-      <c r="G114" s="63" t="s">
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="30"/>
+      <c r="G114" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H114" s="65"/>
-      <c r="I114" s="65"/>
+      <c r="H114" s="29"/>
+      <c r="I114" s="29"/>
     </row>
     <row r="115" spans="1:9" ht="20.25" customHeight="1">
       <c r="A115" s="16">
@@ -2889,17 +2889,17 @@
       <c r="B115" s="21">
         <v>42192</v>
       </c>
-      <c r="C115" s="41" t="s">
+      <c r="C115" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D115" s="42"/>
-      <c r="E115" s="42"/>
-      <c r="F115" s="43"/>
-      <c r="G115" s="63" t="s">
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="30"/>
+      <c r="G115" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H115" s="65"/>
-      <c r="I115" s="65"/>
+      <c r="H115" s="29"/>
+      <c r="I115" s="29"/>
     </row>
     <row r="116" spans="1:9" ht="15" customHeight="1">
       <c r="A116" s="16">
@@ -2908,17 +2908,17 @@
       <c r="B116" s="21">
         <v>42199</v>
       </c>
-      <c r="C116" s="41" t="s">
+      <c r="C116" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D116" s="42"/>
-      <c r="E116" s="42"/>
-      <c r="F116" s="43"/>
-      <c r="G116" s="63" t="s">
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="30"/>
+      <c r="G116" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="H116" s="65"/>
-      <c r="I116" s="65"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
     </row>
     <row r="117" spans="1:9" ht="15" customHeight="1">
       <c r="A117" s="16">
@@ -2927,115 +2927,115 @@
       <c r="B117" s="21">
         <v>42206</v>
       </c>
-      <c r="C117" s="71" t="s">
+      <c r="C117" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="D117" s="72"/>
-      <c r="E117" s="72"/>
-      <c r="F117" s="73"/>
-      <c r="G117" s="63" t="s">
+      <c r="D117" s="32"/>
+      <c r="E117" s="32"/>
+      <c r="F117" s="33"/>
+      <c r="G117" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="H117" s="65"/>
-      <c r="I117" s="65"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
     </row>
     <row r="118" spans="1:9" ht="30" customHeight="1">
       <c r="A118" s="4"/>
     </row>
     <row r="119" spans="1:9" ht="54.75" customHeight="1">
-      <c r="A119" s="56" t="s">
+      <c r="A119" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B119" s="56"/>
-      <c r="C119" s="56"/>
-      <c r="D119" s="56"/>
-      <c r="E119" s="56"/>
-      <c r="F119" s="56"/>
-      <c r="G119" s="56"/>
-      <c r="H119" s="56"/>
-      <c r="I119" s="56"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="39"/>
+      <c r="D119" s="39"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="39"/>
+      <c r="I119" s="39"/>
     </row>
     <row r="120" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A120" s="57" t="s">
+      <c r="A120" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B120" s="58"/>
-      <c r="C120" s="58"/>
-      <c r="D120" s="58"/>
-      <c r="E120" s="58"/>
-      <c r="F120" s="58"/>
-      <c r="G120" s="58"/>
-      <c r="H120" s="58"/>
-      <c r="I120" s="59"/>
+      <c r="B120" s="41"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
+      <c r="E120" s="41"/>
+      <c r="F120" s="41"/>
+      <c r="G120" s="41"/>
+      <c r="H120" s="41"/>
+      <c r="I120" s="42"/>
     </row>
     <row r="121" spans="1:9" ht="30" customHeight="1">
       <c r="A121" s="4"/>
     </row>
     <row r="122" spans="1:9" ht="72" customHeight="1">
-      <c r="A122" s="56" t="s">
+      <c r="A122" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B122" s="56"/>
-      <c r="C122" s="56"/>
-      <c r="D122" s="56"/>
-      <c r="E122" s="56"/>
-      <c r="F122" s="56"/>
-      <c r="G122" s="56"/>
-      <c r="H122" s="56"/>
-      <c r="I122" s="56"/>
+      <c r="B122" s="39"/>
+      <c r="C122" s="39"/>
+      <c r="D122" s="39"/>
+      <c r="E122" s="39"/>
+      <c r="F122" s="39"/>
+      <c r="G122" s="39"/>
+      <c r="H122" s="39"/>
+      <c r="I122" s="39"/>
     </row>
     <row r="123" spans="1:9" ht="15" customHeight="1" thickBot="1">
-      <c r="A123" s="57" t="s">
+      <c r="A123" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B123" s="58"/>
-      <c r="C123" s="58"/>
-      <c r="D123" s="58"/>
-      <c r="E123" s="58"/>
-      <c r="F123" s="58"/>
-      <c r="G123" s="58"/>
-      <c r="H123" s="58"/>
-      <c r="I123" s="59"/>
+      <c r="B123" s="41"/>
+      <c r="C123" s="41"/>
+      <c r="D123" s="41"/>
+      <c r="E123" s="41"/>
+      <c r="F123" s="41"/>
+      <c r="G123" s="41"/>
+      <c r="H123" s="41"/>
+      <c r="I123" s="42"/>
     </row>
     <row r="124" spans="1:9" ht="28.5" customHeight="1">
       <c r="A124" s="4"/>
     </row>
     <row r="125" spans="1:9" ht="127.5" customHeight="1">
-      <c r="A125" s="56" t="s">
+      <c r="A125" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B125" s="56"/>
-      <c r="C125" s="56"/>
-      <c r="D125" s="56"/>
-      <c r="E125" s="56"/>
-      <c r="F125" s="56"/>
-      <c r="G125" s="56"/>
-      <c r="H125" s="56"/>
-      <c r="I125" s="56"/>
+      <c r="B125" s="39"/>
+      <c r="C125" s="39"/>
+      <c r="D125" s="39"/>
+      <c r="E125" s="39"/>
+      <c r="F125" s="39"/>
+      <c r="G125" s="39"/>
+      <c r="H125" s="39"/>
+      <c r="I125" s="39"/>
     </row>
     <row r="126" spans="1:9" ht="333.75" customHeight="1">
-      <c r="A126" s="66" t="s">
+      <c r="A126" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B126" s="66"/>
-      <c r="C126" s="66"/>
-      <c r="D126" s="66"/>
-      <c r="E126" s="66"/>
-      <c r="F126" s="66"/>
-      <c r="G126" s="66"/>
-      <c r="H126" s="66"/>
-      <c r="I126" s="66"/>
+      <c r="B126" s="25"/>
+      <c r="C126" s="25"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="25"/>
+      <c r="F126" s="25"/>
+      <c r="G126" s="25"/>
+      <c r="H126" s="25"/>
+      <c r="I126" s="25"/>
     </row>
     <row r="127" spans="1:9" ht="15" customHeight="1">
-      <c r="A127" s="66"/>
-      <c r="B127" s="66"/>
-      <c r="C127" s="66"/>
-      <c r="D127" s="66"/>
-      <c r="E127" s="66"/>
-      <c r="F127" s="66"/>
-      <c r="G127" s="66"/>
-      <c r="H127" s="66"/>
-      <c r="I127" s="66"/>
+      <c r="A127" s="25"/>
+      <c r="B127" s="25"/>
+      <c r="C127" s="25"/>
+      <c r="D127" s="25"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="25"/>
+      <c r="H127" s="25"/>
+      <c r="I127" s="25"/>
     </row>
     <row r="128" spans="1:9" ht="15.75" customHeight="1">
       <c r="A128" s="4"/>
@@ -5851,6 +5851,91 @@
     </row>
   </sheetData>
   <mergeCells count="109">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A54:I54"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A57:I57"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="A67:I67"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="A71:I71"/>
+    <mergeCell ref="A72:I72"/>
+    <mergeCell ref="A74:I74"/>
+    <mergeCell ref="A75:I75"/>
+    <mergeCell ref="A77:I77"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A83:I83"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="B88:G88"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A96:I96"/>
+    <mergeCell ref="A97:I97"/>
+    <mergeCell ref="A99:I99"/>
+    <mergeCell ref="C101:F101"/>
+    <mergeCell ref="G101:I101"/>
+    <mergeCell ref="C102:F102"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="C103:F103"/>
+    <mergeCell ref="G103:I103"/>
+    <mergeCell ref="C111:F111"/>
+    <mergeCell ref="G111:I111"/>
+    <mergeCell ref="C112:F112"/>
+    <mergeCell ref="G112:I112"/>
+    <mergeCell ref="G113:I113"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G104:I104"/>
+    <mergeCell ref="C106:F106"/>
+    <mergeCell ref="G105:I105"/>
+    <mergeCell ref="C107:F107"/>
+    <mergeCell ref="G106:I106"/>
+    <mergeCell ref="G107:I107"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="G108:I108"/>
     <mergeCell ref="A126:I127"/>
     <mergeCell ref="H63:J63"/>
     <mergeCell ref="H64:J64"/>
@@ -5875,91 +5960,6 @@
     <mergeCell ref="G109:I109"/>
     <mergeCell ref="C110:F110"/>
     <mergeCell ref="G110:I110"/>
-    <mergeCell ref="C111:F111"/>
-    <mergeCell ref="G111:I111"/>
-    <mergeCell ref="C112:F112"/>
-    <mergeCell ref="G112:I112"/>
-    <mergeCell ref="G113:I113"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G104:I104"/>
-    <mergeCell ref="C106:F106"/>
-    <mergeCell ref="G105:I105"/>
-    <mergeCell ref="C107:F107"/>
-    <mergeCell ref="G106:I106"/>
-    <mergeCell ref="G107:I107"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="G108:I108"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A96:I96"/>
-    <mergeCell ref="A97:I97"/>
-    <mergeCell ref="A99:I99"/>
-    <mergeCell ref="C101:F101"/>
-    <mergeCell ref="G101:I101"/>
-    <mergeCell ref="C102:F102"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="C103:F103"/>
-    <mergeCell ref="G103:I103"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A83:I83"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="B88:G88"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="A67:I67"/>
-    <mergeCell ref="A69:I69"/>
-    <mergeCell ref="A71:I71"/>
-    <mergeCell ref="A72:I72"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="A75:I75"/>
-    <mergeCell ref="A77:I77"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="A57:I57"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A60:I60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:I12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A26" r:id="rId1"/>

</xml_diff>